<commit_message>
Added subtraction to correct Table 10
</commit_message>
<xml_diff>
--- a/SDGEGRC24/TURN-SEU-031_ATTACH_Q1a_10493_10492_UGCCCircuitRisk_jwm.xlsx
+++ b/SDGEGRC24/TURN-SEU-031_ATTACH_Q1a_10493_10492_UGCCCircuitRisk_jwm.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D94396F-C384-2849-8745-ECBB98DA1495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A83CA64-EF86-054D-88E4-BB0907D46A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-880" yWindow="-20600" windowWidth="35840" windowHeight="20600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="500" windowWidth="35840" windowHeight="20580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1a_sup_1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3136" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="806">
   <si>
     <t>segment</t>
   </si>
@@ -2442,6 +2442,12 @@
   </si>
   <si>
     <t>Total Risk</t>
+  </si>
+  <si>
+    <t>WF Mit Risk</t>
+  </si>
+  <si>
+    <t>PSPS Mit Risk</t>
   </si>
 </sst>
 </file>
@@ -2543,7 +2549,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -2853,7 +2859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G635"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A596" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
+    <sheetView topLeftCell="A599" zoomScale="101" zoomScaleNormal="101" workbookViewId="0">
       <selection activeCell="E637" sqref="E637"/>
     </sheetView>
   </sheetViews>
@@ -17890,10 +17896,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G589"/>
+  <dimension ref="A1:J589"/>
   <sheetViews>
-    <sheetView topLeftCell="A553" workbookViewId="0">
-      <selection activeCell="E587" sqref="E587:F589"/>
+    <sheetView tabSelected="1" topLeftCell="A557" workbookViewId="0">
+      <selection activeCell="M587" sqref="M587"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17905,6 +17911,7 @@
     <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -31668,7 +31675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="577" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>605</v>
       </c>
@@ -31692,7 +31699,7 @@
         <v>2.4118901609768969E-5</v>
       </c>
     </row>
-    <row r="578" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
         <v>589</v>
       </c>
@@ -31716,7 +31723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="579" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
         <v>601</v>
       </c>
@@ -31740,7 +31747,7 @@
         <v>1.946204841583305E-5</v>
       </c>
     </row>
-    <row r="581" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C581" t="s">
         <v>794</v>
       </c>
@@ -31753,8 +31760,14 @@
       <c r="G581" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="582" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I581" t="s">
+        <v>804</v>
+      </c>
+      <c r="J581" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="582" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C582">
         <f>SUM(C5:C579)</f>
         <v>1.4979999999999985E-2</v>
@@ -31771,8 +31784,16 @@
         <f>SUM(G5:G579)</f>
         <v>2.1449753836573484E-3</v>
       </c>
-    </row>
-    <row r="584" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I582">
+        <f>C582-F582</f>
+        <v>1.1324999999999984E-2</v>
+      </c>
+      <c r="J582">
+        <f>D582-G582</f>
+        <v>2.2508155731271419E-3</v>
+      </c>
+    </row>
+    <row r="584" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E584" t="s">
         <v>798</v>
       </c>
@@ -31781,7 +31802,7 @@
         <v>0.75600801068090762</v>
       </c>
     </row>
-    <row r="585" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E585" t="s">
         <v>799</v>
       </c>
@@ -31790,7 +31811,7 @@
         <v>0.48796118940705779</v>
       </c>
     </row>
-    <row r="587" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E587" t="s">
         <v>803</v>
       </c>
@@ -31799,7 +31820,7 @@
         <v>1.9375790956784475E-2</v>
       </c>
     </row>
-    <row r="588" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E588" t="s">
         <v>802</v>
       </c>
@@ -31808,7 +31829,7 @@
         <v>0.58449226796775033</v>
       </c>
     </row>
-    <row r="589" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E589" t="s">
         <v>801</v>
       </c>
@@ -31827,7 +31848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
@@ -35528,37 +35549,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PartyFullName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">
-      <Value>303</Value>
-    </PartyFullName>
-    <PDRNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">PDR_P987</PDRNumber>
-    <DocumentType xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">Final Attachment</DocumentType>
-    <DocketNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">A2205015_016 2024 GRC</DocketNumber>
-    <RequestorName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">
-      <Value>355</Value>
-    </RequestorName>
-    <ProceedingName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">53</ProceedingName>
-    <GroupNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">R3111_Group1</GroupNumber>
-    <SourceType xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">Workflow Library</SourceType>
-    <DataRequestNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">TURN-SEU-031 </DataRequestNumber>
-    <PublishedBy xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">SDGE and SoCalGas</PublishedBy>
-    <PublishedTo xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">SDGE and SoCalGas</PublishedTo>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Discovery Data Response Library" ma:contentTypeID="0x01010078A1A4D929017144A85790D17785142400EE6E0270FB7F5B4C97E888C45758AD26" ma:contentTypeVersion="15" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="0dfeabb7de1a23bedf8e0d905c57112f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12174cd8-9950-459c-a1a6-43cfa5072f14" xmlns:ns3="f7575cc7-459e-4e34-97b6-1e875b6f85c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fa05a21ff3d6d450c770fa9c2103a52" ns2:_="" ns3:_="">
     <xsd:import namespace="12174cd8-9950-459c-a1a6-43cfa5072f14"/>
@@ -35827,25 +35817,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5BB9B9-D0B5-4544-9DD4-CDF3F4438C7C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12174cd8-9950-459c-a1a6-43cfa5072f14"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37465A-8BB6-4C68-8862-A088DF271882}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PartyFullName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">
+      <Value>303</Value>
+    </PartyFullName>
+    <PDRNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">PDR_P987</PDRNumber>
+    <DocumentType xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">Final Attachment</DocumentType>
+    <DocketNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">A2205015_016 2024 GRC</DocketNumber>
+    <RequestorName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">
+      <Value>355</Value>
+    </RequestorName>
+    <ProceedingName xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">53</ProceedingName>
+    <GroupNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">R3111_Group1</GroupNumber>
+    <SourceType xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">Workflow Library</SourceType>
+    <DataRequestNumber xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">TURN-SEU-031 </DataRequestNumber>
+    <PublishedBy xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">SDGE and SoCalGas</PublishedBy>
+    <PublishedTo xmlns="12174cd8-9950-459c-a1a6-43cfa5072f14">SDGE and SoCalGas</PublishedTo>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF55FD2-E964-4232-BB44-010553785F22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -35862,4 +35865,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A37465A-8BB6-4C68-8862-A088DF271882}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5BB9B9-D0B5-4544-9DD4-CDF3F4438C7C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12174cd8-9950-459c-a1a6-43cfa5072f14"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>